<commit_message>
A: add slides and new versions
</commit_message>
<xml_diff>
--- a/HW1/Applied Electronics Data.xlsx
+++ b/HW1/Applied Electronics Data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emory-my.sharepoint.com/personal/rli328_emory_edu/Documents/Spring_Optimization/HW/HW1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emory-my.sharepoint.com/personal/rli328_emory_edu/Documents/Spring_Optimization/Oprimization_HW/HW1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{3B047C91-0ABE-455B-97EB-921524713510}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{347816CD-A67F-E343-8478-E27BF1AEBC7E}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{3B047C91-0ABE-455B-97EB-921524713510}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A316BA6A-A75A-1047-A8DF-85C45A8DAFAE}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -352,10 +352,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -621,8 +617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="138" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="138" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16"/>

</xml_diff>